<commit_message>
Add FOREIGN KEY (animal_id) for table outcome.
</commit_message>
<xml_diff>
--- a/sketch.xlsx
+++ b/sketch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <r>
       <t>'name'</t>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -915,6 +915,9 @@
       </c>
       <c r="P19" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:17">

</xml_diff>